<commit_message>
updating analysis result on the mRNA de novo sequencing
</commit_message>
<xml_diff>
--- a/coverage_summary_long.xlsx
+++ b/coverage_summary_long.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rt753149/Desktop/mRNA_sequencing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shangsilin/Desktop/Autumn 2025/mRNA_sequencing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD80DC27-B550-814F-9C7C-7AA9603B536C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21356CF1-95C0-FA4D-948A-22C2F981A66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -284,15 +284,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -593,15 +588,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="114" workbookViewId="0">
-      <selection activeCell="U43" sqref="U43"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
     <col min="2" max="51" width="3.83203125" customWidth="1"/>
-    <col min="52" max="52" width="3" style="11" customWidth="1"/>
+    <col min="52" max="52" width="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -755,7 +750,6 @@
       <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="9"/>
     </row>
     <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -911,7 +905,7 @@
       <c r="AY2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AZ2" s="10"/>
+      <c r="AZ2" s="6"/>
     </row>
     <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1067,7 +1061,7 @@
       <c r="AY3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ3" s="10"/>
+      <c r="AZ3" s="6"/>
     </row>
     <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1223,7 +1217,7 @@
       <c r="AY4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ4" s="10"/>
+      <c r="AZ4" s="6"/>
     </row>
     <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1379,7 +1373,7 @@
       <c r="AY5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AZ5" s="10"/>
+      <c r="AZ5" s="6"/>
     </row>
     <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1400,13 +1394,13 @@
       <c r="F6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="G6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>51</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -1535,7 +1529,7 @@
       <c r="AY6" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ6" s="10"/>
+      <c r="AZ6" s="6"/>
     </row>
     <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1691,7 +1685,7 @@
       <c r="AY7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AZ7" s="10"/>
+      <c r="AZ7" s="6"/>
     </row>
     <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1847,7 +1841,7 @@
       <c r="AY8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ8" s="10"/>
+      <c r="AZ8" s="6"/>
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -2003,7 +1997,7 @@
       <c r="AY9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AZ9" s="10"/>
+      <c r="AZ9" s="6"/>
     </row>
     <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -2159,7 +2153,7 @@
       <c r="AY10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ10" s="10"/>
+      <c r="AZ10" s="6"/>
     </row>
     <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -2315,7 +2309,7 @@
       <c r="AY11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AZ11" s="10"/>
+      <c r="AZ11" s="6"/>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -2471,7 +2465,7 @@
       <c r="AY12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ12" s="10"/>
+      <c r="AZ12" s="6"/>
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -2627,7 +2621,7 @@
       <c r="AY13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AZ13" s="10"/>
+      <c r="AZ13" s="6"/>
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -2783,7 +2777,7 @@
       <c r="AY14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AZ14" s="10"/>
+      <c r="AZ14" s="6"/>
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -2939,7 +2933,7 @@
       <c r="AY15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ15" s="10"/>
+      <c r="AZ15" s="6"/>
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -3095,7 +3089,7 @@
       <c r="AY16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AZ16" s="10"/>
+      <c r="AZ16" s="6"/>
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -3251,7 +3245,7 @@
       <c r="AY17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ17" s="10"/>
+      <c r="AZ17" s="6"/>
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -3407,7 +3401,7 @@
       <c r="AY18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AZ18" s="10"/>
+      <c r="AZ18" s="6"/>
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -3563,7 +3557,7 @@
       <c r="AY19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AZ19" s="10"/>
+      <c r="AZ19" s="6"/>
     </row>
     <row r="20" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -3719,7 +3713,7 @@
       <c r="AY20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AZ20" s="10"/>
+      <c r="AZ20" s="6"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -3824,13 +3818,13 @@
       <c r="AH21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AI21" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK21" s="4" t="s">
+      <c r="AI21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK21" s="3" t="s">
         <v>51</v>
       </c>
       <c r="AL21" s="4" t="s">
@@ -3875,7 +3869,7 @@
       <c r="AY21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ21" s="10"/>
+      <c r="AZ21" s="6"/>
     </row>
     <row r="22" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -4031,7 +4025,7 @@
       <c r="AY22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AZ22" s="10"/>
+      <c r="AZ22" s="6"/>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -4187,7 +4181,7 @@
       <c r="AY23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AZ23" s="10"/>
+      <c r="AZ23" s="6"/>
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -4343,7 +4337,7 @@
       <c r="AY24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ24" s="10"/>
+      <c r="AZ24" s="6"/>
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -4499,7 +4493,7 @@
       <c r="AY25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ25" s="10"/>
+      <c r="AZ25" s="6"/>
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -4655,7 +4649,7 @@
       <c r="AY26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ26" s="10"/>
+      <c r="AZ26" s="6"/>
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -4811,7 +4805,7 @@
       <c r="AY27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AZ27" s="10"/>
+      <c r="AZ27" s="6"/>
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -4967,7 +4961,7 @@
       <c r="AY28" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AZ28" s="10"/>
+      <c r="AZ28" s="6"/>
     </row>
     <row r="29" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -5123,7 +5117,7 @@
       <c r="AY29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AZ29" s="10"/>
+      <c r="AZ29" s="6"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -5279,7 +5273,7 @@
       <c r="AY30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ30" s="10"/>
+      <c r="AZ30" s="6"/>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -5435,7 +5429,7 @@
       <c r="AY31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AZ31" s="10"/>
+      <c r="AZ31" s="6"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -5591,7 +5585,7 @@
       <c r="AY32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ32" s="10"/>
+      <c r="AZ32" s="6"/>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -5747,7 +5741,7 @@
       <c r="AY33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ33" s="10"/>
+      <c r="AZ33" s="6"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -5903,7 +5897,7 @@
       <c r="AY34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AZ34" s="10"/>
+      <c r="AZ34" s="6"/>
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -6059,7 +6053,7 @@
       <c r="AY35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ35" s="10"/>
+      <c r="AZ35" s="6"/>
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -6215,7 +6209,7 @@
       <c r="AY36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ36" s="10"/>
+      <c r="AZ36" s="6"/>
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -6371,7 +6365,7 @@
       <c r="AY37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AZ37" s="10"/>
+      <c r="AZ37" s="6"/>
     </row>
     <row r="38" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -6527,7 +6521,7 @@
       <c r="AY38" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AZ38" s="10"/>
+      <c r="AZ38" s="6"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -6683,7 +6677,7 @@
       <c r="AY39" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AZ39" s="10"/>
+      <c r="AZ39" s="6"/>
     </row>
     <row r="40" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -6821,23 +6815,23 @@
       <c r="AW40" s="6"/>
       <c r="AX40" s="6"/>
       <c r="AY40" s="6"/>
-      <c r="AZ40" s="10"/>
+      <c r="AZ40" s="6"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="AC41" s="12"/>
-      <c r="AD41" s="15" t="s">
+      <c r="AC41" s="9"/>
+      <c r="AD41" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="AC42" s="13"/>
+      <c r="AC42" s="10"/>
       <c r="AD42" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.2">
-      <c r="AC43" s="14"/>
-      <c r="AD43" s="15" t="s">
+      <c r="AC43" s="11"/>
+      <c r="AD43" s="12" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>